<commit_message>
atualizada tabelas do banco (excel)
</commit_message>
<xml_diff>
--- a/Banco_de_dados/tabelas.xlsx
+++ b/Banco_de_dados/tabelas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\OneDrive\Documentos\GitHub\ERP_BarberBross\Banco_de_dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4F81F10-FBCD-48E9-B365-8134723AD727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A77C360-5244-4A63-BD3F-02C4891A9D9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="862" activeTab="15" xr2:uid="{671AE30B-6C9B-46EB-A746-2358A445F00B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="862" firstSheet="2" activeTab="15" xr2:uid="{671AE30B-6C9B-46EB-A746-2358A445F00B}"/>
   </bookViews>
   <sheets>
     <sheet name="Empresa" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="446">
   <si>
     <t>Produto</t>
   </si>
@@ -66,9 +66,6 @@
     <t>tipo_assinatura</t>
   </si>
   <si>
-    <t>barbearia_id</t>
-  </si>
-  <si>
     <t>funcinonario_id</t>
   </si>
   <si>
@@ -111,9 +108,6 @@
     <t xml:space="preserve"> cliente_id</t>
   </si>
   <si>
-    <t xml:space="preserve"> barbearia_id</t>
-  </si>
-  <si>
     <t xml:space="preserve"> servico_id</t>
   </si>
   <si>
@@ -1381,6 +1375,9 @@
   </si>
   <si>
     <t>https://instagram.com/barbearia10</t>
+  </si>
+  <si>
+    <t>empresa_id</t>
   </si>
 </sst>
 </file>
@@ -1388,7 +1385,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -1421,35 +1418,35 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
     <dxf>
-      <numFmt numFmtId="168" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+      <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+      <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+      <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+      <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+      <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+      <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+      <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+      <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1468,7 +1465,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{3B466947-9227-4343-9756-FFAB80C2DBB9}" name="Tabela3" displayName="Tabela3" ref="A1:H11" totalsRowShown="0">
   <autoFilter ref="A1:H11" xr:uid="{3B466947-9227-4343-9756-FFAB80C2DBB9}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{8D0769D9-D5D2-4160-80E1-70D4ECBDC3A0}" name="barbearia_id"/>
+    <tableColumn id="1" xr3:uid="{8D0769D9-D5D2-4160-80E1-70D4ECBDC3A0}" name="empresa_id"/>
     <tableColumn id="2" xr3:uid="{D4B97213-6299-42BF-BCEE-2EE531364DE2}" name="razao_social"/>
     <tableColumn id="4" xr3:uid="{D280116C-96ED-48E4-9229-D0C4870E6C98}" name="nome_fantasia"/>
     <tableColumn id="5" xr3:uid="{CB4D2E55-A603-4F2A-8694-A1A457C6AD44}" name="endereco_id"/>
@@ -1515,7 +1512,7 @@
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{28AC5AF0-C532-47BC-9641-0D01D5E803DA}" name="avaliacao_id"/>
     <tableColumn id="2" xr3:uid="{F86245A6-FAEE-4E90-B1EF-F49BD18E6A67}" name=" cliente_id"/>
-    <tableColumn id="3" xr3:uid="{8AF59656-CDC4-45E1-B2E1-6CA80165318A}" name=" funcionario_id"/>
+    <tableColumn id="3" xr3:uid="{8AF59656-CDC4-45E1-B2E1-6CA80165318A}" name="empresa_id"/>
     <tableColumn id="4" xr3:uid="{9A06B760-C5EF-40A7-838E-FCA83A2EDF4B}" name=" servico_id"/>
     <tableColumn id="5" xr3:uid="{EA40A5C3-6D76-45CC-9CCA-7B7927C1E360}" name=" nota"/>
     <tableColumn id="6" xr3:uid="{A24B42C5-8BEF-416B-A99A-C3678E89BDEB}" name=" comentario"/>
@@ -1588,7 +1585,7 @@
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{DC046B78-E0F6-42E0-AFD3-A064CF7A6385}" name="funcinonario_id"/>
     <tableColumn id="2" xr3:uid="{F8563926-DD13-40D0-B6D9-5D624F864213}" name="cpf_cnpj"/>
-    <tableColumn id="3" xr3:uid="{795DAE9E-3D3E-4758-BB27-5DE8564AA6F5}" name="barbearia_id"/>
+    <tableColumn id="3" xr3:uid="{795DAE9E-3D3E-4758-BB27-5DE8564AA6F5}" name="empresa_id"/>
     <tableColumn id="4" xr3:uid="{2C1F7484-FA07-4E56-B8C3-BDF75791F4D8}" name="nome"/>
     <tableColumn id="5" xr3:uid="{370D8C95-AFA6-4320-BF88-98C5BE110789}" name="nome_social"/>
     <tableColumn id="6" xr3:uid="{60A7EE17-570E-4E5F-820D-82F7D94E039D}" name="email"/>
@@ -1628,17 +1625,18 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{BC5EDE39-B857-4EEE-AE56-3DB436B1C5D9}" name="Tabela8" displayName="Tabela8" ref="A1:H11" totalsRowShown="0">
-  <autoFilter ref="A1:H11" xr:uid="{BC5EDE39-B857-4EEE-AE56-3DB436B1C5D9}"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{BC5EDE39-B857-4EEE-AE56-3DB436B1C5D9}" name="Tabela8" displayName="Tabela8" ref="A1:I11" totalsRowShown="0">
+  <autoFilter ref="A1:I11" xr:uid="{BC5EDE39-B857-4EEE-AE56-3DB436B1C5D9}"/>
+  <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{3AA616EC-45C7-42C9-B78B-B52358880C80}" name="agendamento_id"/>
     <tableColumn id="2" xr3:uid="{F4E53F3A-9473-4E39-AD13-C8E269B6716D}" name=" data_hora"/>
     <tableColumn id="3" xr3:uid="{9E86F784-54A7-4AE4-AF7A-F07D6FEFEF78}" name=" cliente_id"/>
-    <tableColumn id="4" xr3:uid="{231ECE45-D33C-4A2C-8E40-3A1BFEDFC314}" name=" barbearia_id"/>
+    <tableColumn id="4" xr3:uid="{231ECE45-D33C-4A2C-8E40-3A1BFEDFC314}" name="empresa_id"/>
     <tableColumn id="5" xr3:uid="{AAB95E63-E776-436D-9EEE-39AFF14A7418}" name=" servico_id"/>
     <tableColumn id="6" xr3:uid="{7373331B-DDC2-4BF5-A755-BDC7CABE883B}" name=" status"/>
     <tableColumn id="7" xr3:uid="{49BB69B3-40EF-4E3C-8E93-DDFEE4E3862F}" name=" observação"/>
     <tableColumn id="8" xr3:uid="{3D60C77C-6593-4459-809B-887C44C54492}" name=" preco_id"/>
+    <tableColumn id="9" xr3:uid="{51D3F2DD-1048-4F08-B271-0D727841D450}" name="funcionario_id"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2002,9 +2000,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A24D2798-F6CD-4152-856C-AEB17176CEF3}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2020,7 +2016,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>445</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -2049,25 +2045,25 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" t="s">
         <v>74</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>75</v>
-      </c>
-      <c r="G2" t="s">
-        <v>76</v>
-      </c>
-      <c r="H2" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -2075,25 +2071,25 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D3">
         <v>2</v>
       </c>
       <c r="E3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G3" t="s">
         <v>80</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>81</v>
-      </c>
-      <c r="G3" t="s">
-        <v>82</v>
-      </c>
-      <c r="H3" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -2101,25 +2097,25 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D4">
         <v>3</v>
       </c>
       <c r="E4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G4" t="s">
         <v>86</v>
       </c>
-      <c r="F4" t="s">
-        <v>87</v>
-      </c>
-      <c r="G4" t="s">
-        <v>88</v>
-      </c>
       <c r="H4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -2127,25 +2123,25 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D5">
         <v>4</v>
       </c>
       <c r="E5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F5" t="s">
+        <v>90</v>
+      </c>
+      <c r="G5" t="s">
         <v>91</v>
       </c>
-      <c r="F5" t="s">
+      <c r="H5" t="s">
         <v>92</v>
-      </c>
-      <c r="G5" t="s">
-        <v>93</v>
-      </c>
-      <c r="H5" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -2153,25 +2149,25 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D6">
         <v>5</v>
       </c>
       <c r="E6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F6" t="s">
+        <v>96</v>
+      </c>
+      <c r="G6" t="s">
         <v>97</v>
       </c>
-      <c r="F6" t="s">
-        <v>98</v>
-      </c>
-      <c r="G6" t="s">
-        <v>99</v>
-      </c>
       <c r="H6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -2179,25 +2175,25 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D7">
         <v>6</v>
       </c>
       <c r="E7" t="s">
+        <v>100</v>
+      </c>
+      <c r="F7" t="s">
+        <v>101</v>
+      </c>
+      <c r="G7" t="s">
         <v>102</v>
       </c>
-      <c r="F7" t="s">
-        <v>103</v>
-      </c>
-      <c r="G7" t="s">
-        <v>104</v>
-      </c>
       <c r="H7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -2205,25 +2201,25 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D8">
         <v>7</v>
       </c>
       <c r="E8" t="s">
+        <v>105</v>
+      </c>
+      <c r="F8" t="s">
+        <v>106</v>
+      </c>
+      <c r="G8" t="s">
         <v>107</v>
       </c>
-      <c r="F8" t="s">
-        <v>108</v>
-      </c>
-      <c r="G8" t="s">
-        <v>109</v>
-      </c>
       <c r="H8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -2231,25 +2227,25 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D9">
         <v>8</v>
       </c>
       <c r="E9" t="s">
+        <v>110</v>
+      </c>
+      <c r="F9" t="s">
+        <v>111</v>
+      </c>
+      <c r="G9" t="s">
         <v>112</v>
       </c>
-      <c r="F9" t="s">
-        <v>113</v>
-      </c>
-      <c r="G9" t="s">
-        <v>114</v>
-      </c>
       <c r="H9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -2257,25 +2253,25 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D10">
         <v>9</v>
       </c>
       <c r="E10" t="s">
+        <v>115</v>
+      </c>
+      <c r="F10" t="s">
+        <v>116</v>
+      </c>
+      <c r="G10" t="s">
         <v>117</v>
       </c>
-      <c r="F10" t="s">
-        <v>118</v>
-      </c>
-      <c r="G10" t="s">
-        <v>119</v>
-      </c>
       <c r="H10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -2283,25 +2279,25 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C11" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D11">
         <v>10</v>
       </c>
       <c r="E11" t="s">
+        <v>120</v>
+      </c>
+      <c r="F11" t="s">
+        <v>121</v>
+      </c>
+      <c r="G11" t="s">
         <v>122</v>
       </c>
-      <c r="F11" t="s">
-        <v>123</v>
-      </c>
-      <c r="G11" t="s">
-        <v>124</v>
-      </c>
       <c r="H11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -2330,16 +2326,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -2347,10 +2343,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C2" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -2361,10 +2357,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C3" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -2375,13 +2371,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C4" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="D4" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -2389,10 +2385,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C5" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
@@ -2403,13 +2399,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C6" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D6" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -2417,10 +2413,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C7" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
@@ -2431,13 +2427,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C8" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D8" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -2445,10 +2441,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C9" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D9" t="s">
         <v>0</v>
@@ -2459,13 +2455,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C10" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="D10" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -2473,13 +2469,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C11" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="D11" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
   </sheetData>
@@ -2510,22 +2506,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" t="s">
         <v>47</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>48</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" t="s">
         <v>49</v>
-      </c>
-      <c r="D1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -2539,13 +2535,13 @@
         <v>45915</v>
       </c>
       <c r="D2" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="E2" s="1">
         <v>45915.041666666657</v>
       </c>
       <c r="F2" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -2559,13 +2555,13 @@
         <v>45916</v>
       </c>
       <c r="D3" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E3" s="1">
         <v>45916.041666666657</v>
       </c>
       <c r="F3" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -2579,13 +2575,13 @@
         <v>45917</v>
       </c>
       <c r="D4" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="E4" s="1">
         <v>45917.041666666657</v>
       </c>
       <c r="F4" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -2599,13 +2595,13 @@
         <v>45918</v>
       </c>
       <c r="D5" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="E5" s="1">
         <v>45918.041666666657</v>
       </c>
       <c r="F5" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -2619,13 +2615,13 @@
         <v>45919</v>
       </c>
       <c r="D6" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="E6" s="1">
         <v>45919.041666666657</v>
       </c>
       <c r="F6" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -2639,13 +2635,13 @@
         <v>45920</v>
       </c>
       <c r="D7" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="E7" s="1">
         <v>45920.041666666657</v>
       </c>
       <c r="F7" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -2659,13 +2655,13 @@
         <v>45921</v>
       </c>
       <c r="D8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E8" s="1">
         <v>45921.041666666657</v>
       </c>
       <c r="F8" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -2679,13 +2675,13 @@
         <v>45922</v>
       </c>
       <c r="D9" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="E9" s="1">
         <v>45922.041666666657</v>
       </c>
       <c r="F9" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -2699,13 +2695,13 @@
         <v>45923</v>
       </c>
       <c r="D10" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="E10" s="1">
         <v>45923.041666666657</v>
       </c>
       <c r="F10" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -2719,13 +2715,13 @@
         <v>45924</v>
       </c>
       <c r="D11" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="E11" s="1">
         <v>45924.041666666657</v>
       </c>
       <c r="F11" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
   </sheetData>
@@ -2741,7 +2737,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G11"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2757,25 +2753,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>445</v>
+      </c>
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" t="s">
         <v>52</v>
       </c>
-      <c r="B1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F1" t="s">
-        <v>54</v>
-      </c>
       <c r="G1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -2795,7 +2791,7 @@
         <v>5</v>
       </c>
       <c r="F2" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="G2" s="1">
         <v>45901</v>
@@ -2818,7 +2814,7 @@
         <v>3</v>
       </c>
       <c r="F3" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="G3" s="1">
         <v>45902</v>
@@ -2841,7 +2837,7 @@
         <v>3</v>
       </c>
       <c r="F4" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="G4" s="1">
         <v>45903</v>
@@ -2864,7 +2860,7 @@
         <v>3</v>
       </c>
       <c r="F5" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="G5" s="1">
         <v>45904</v>
@@ -2887,7 +2883,7 @@
         <v>4</v>
       </c>
       <c r="F6" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="G6" s="1">
         <v>45905</v>
@@ -2910,7 +2906,7 @@
         <v>4</v>
       </c>
       <c r="F7" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="G7" s="1">
         <v>45906</v>
@@ -2933,7 +2929,7 @@
         <v>4</v>
       </c>
       <c r="F8" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="G8" s="1">
         <v>45907</v>
@@ -2956,7 +2952,7 @@
         <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="G9" s="1">
         <v>45908</v>
@@ -2979,7 +2975,7 @@
         <v>2</v>
       </c>
       <c r="F10" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="G10" s="1">
         <v>45909</v>
@@ -3002,7 +2998,7 @@
         <v>3</v>
       </c>
       <c r="F11" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="G11" s="1">
         <v>45910</v>
@@ -3035,22 +3031,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" t="s">
         <v>55</v>
       </c>
-      <c r="B1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>56</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>57</v>
-      </c>
-      <c r="E1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -3058,7 +3054,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -3078,7 +3074,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C3">
         <v>6</v>
@@ -3098,7 +3094,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -3118,7 +3114,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -3138,7 +3134,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -3158,7 +3154,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -3178,7 +3174,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C8">
         <v>4</v>
@@ -3198,7 +3194,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C9">
         <v>4</v>
@@ -3218,7 +3214,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -3238,7 +3234,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C11">
         <v>9</v>
@@ -3281,22 +3277,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" t="s">
         <v>60</v>
       </c>
-      <c r="B1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>61</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>62</v>
-      </c>
-      <c r="E1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -3304,16 +3300,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>392</v>
+      </c>
+      <c r="C2" t="s">
+        <v>393</v>
+      </c>
+      <c r="D2" t="s">
         <v>394</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>395</v>
-      </c>
-      <c r="D2" t="s">
-        <v>396</v>
-      </c>
-      <c r="E2" t="s">
-        <v>397</v>
       </c>
       <c r="F2">
         <v>7</v>
@@ -3324,16 +3320,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>396</v>
+      </c>
+      <c r="C3" t="s">
+        <v>397</v>
+      </c>
+      <c r="D3" t="s">
         <v>398</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>399</v>
-      </c>
-      <c r="D3" t="s">
-        <v>400</v>
-      </c>
-      <c r="E3" t="s">
-        <v>401</v>
       </c>
       <c r="F3">
         <v>7</v>
@@ -3344,16 +3340,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>400</v>
+      </c>
+      <c r="C4" t="s">
+        <v>401</v>
+      </c>
+      <c r="D4" t="s">
         <v>402</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>403</v>
-      </c>
-      <c r="D4" t="s">
-        <v>404</v>
-      </c>
-      <c r="E4" t="s">
-        <v>405</v>
       </c>
       <c r="F4">
         <v>10</v>
@@ -3364,16 +3360,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>404</v>
+      </c>
+      <c r="C5" t="s">
+        <v>405</v>
+      </c>
+      <c r="D5" t="s">
         <v>406</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
         <v>407</v>
-      </c>
-      <c r="D5" t="s">
-        <v>408</v>
-      </c>
-      <c r="E5" t="s">
-        <v>409</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -3384,16 +3380,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>408</v>
+      </c>
+      <c r="C6" t="s">
+        <v>409</v>
+      </c>
+      <c r="D6" t="s">
         <v>410</v>
       </c>
-      <c r="C6" t="s">
+      <c r="E6" t="s">
         <v>411</v>
-      </c>
-      <c r="D6" t="s">
-        <v>412</v>
-      </c>
-      <c r="E6" t="s">
-        <v>413</v>
       </c>
       <c r="F6">
         <v>5</v>
@@ -3404,16 +3400,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>412</v>
+      </c>
+      <c r="C7" t="s">
+        <v>413</v>
+      </c>
+      <c r="D7" t="s">
         <v>414</v>
       </c>
-      <c r="C7" t="s">
+      <c r="E7" t="s">
         <v>415</v>
-      </c>
-      <c r="D7" t="s">
-        <v>416</v>
-      </c>
-      <c r="E7" t="s">
-        <v>417</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -3424,16 +3420,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>416</v>
+      </c>
+      <c r="C8" t="s">
+        <v>417</v>
+      </c>
+      <c r="D8" t="s">
         <v>418</v>
       </c>
-      <c r="C8" t="s">
+      <c r="E8" t="s">
         <v>419</v>
-      </c>
-      <c r="D8" t="s">
-        <v>420</v>
-      </c>
-      <c r="E8" t="s">
-        <v>421</v>
       </c>
       <c r="F8">
         <v>10</v>
@@ -3444,16 +3440,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>420</v>
+      </c>
+      <c r="C9" t="s">
+        <v>421</v>
+      </c>
+      <c r="D9" t="s">
         <v>422</v>
       </c>
-      <c r="C9" t="s">
+      <c r="E9" t="s">
         <v>423</v>
-      </c>
-      <c r="D9" t="s">
-        <v>424</v>
-      </c>
-      <c r="E9" t="s">
-        <v>425</v>
       </c>
       <c r="F9">
         <v>1</v>
@@ -3464,16 +3460,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>424</v>
+      </c>
+      <c r="C10" t="s">
+        <v>425</v>
+      </c>
+      <c r="D10" t="s">
         <v>426</v>
       </c>
-      <c r="C10" t="s">
+      <c r="E10" t="s">
         <v>427</v>
-      </c>
-      <c r="D10" t="s">
-        <v>428</v>
-      </c>
-      <c r="E10" t="s">
-        <v>429</v>
       </c>
       <c r="F10">
         <v>3</v>
@@ -3484,16 +3480,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>428</v>
+      </c>
+      <c r="C11" t="s">
+        <v>429</v>
+      </c>
+      <c r="D11" t="s">
         <v>430</v>
       </c>
-      <c r="C11" t="s">
+      <c r="E11" t="s">
         <v>431</v>
-      </c>
-      <c r="D11" t="s">
-        <v>432</v>
-      </c>
-      <c r="E11" t="s">
-        <v>433</v>
       </c>
       <c r="F11">
         <v>7</v>
@@ -3527,22 +3523,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" t="s">
         <v>65</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>66</v>
       </c>
-      <c r="C1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E1" t="s">
-        <v>68</v>
-      </c>
       <c r="F1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -3559,10 +3555,10 @@
         <v>45905</v>
       </c>
       <c r="E2" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="F2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -3579,10 +3575,10 @@
         <v>45906</v>
       </c>
       <c r="E3" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="F3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -3599,10 +3595,10 @@
         <v>45907</v>
       </c>
       <c r="E4" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="F4" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -3619,10 +3615,10 @@
         <v>45908</v>
       </c>
       <c r="E5" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="F5" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -3639,10 +3635,10 @@
         <v>45909</v>
       </c>
       <c r="E6" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="F6" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -3659,10 +3655,10 @@
         <v>45910</v>
       </c>
       <c r="E7" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="F7" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -3679,10 +3675,10 @@
         <v>45911</v>
       </c>
       <c r="E8" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="F8" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -3699,10 +3695,10 @@
         <v>45912</v>
       </c>
       <c r="E9" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="F9" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -3719,10 +3715,10 @@
         <v>45913</v>
       </c>
       <c r="E10" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="F10" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -3739,10 +3735,10 @@
         <v>45914</v>
       </c>
       <c r="E11" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="F11" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
   </sheetData>
@@ -3758,7 +3754,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C11"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3770,13 +3766,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" t="s">
         <v>69</v>
-      </c>
-      <c r="B1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -3784,7 +3780,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C2">
         <v>4</v>
@@ -3795,7 +3791,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C3">
         <v>10</v>
@@ -3806,7 +3802,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="C4">
         <v>4</v>
@@ -3817,7 +3813,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C5">
         <v>7</v>
@@ -3828,7 +3824,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="C6">
         <v>8</v>
@@ -3839,7 +3835,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -3850,7 +3846,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -3861,7 +3857,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="C9">
         <v>4</v>
@@ -3872,7 +3868,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C10">
         <v>7</v>
@@ -3883,7 +3879,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="C11">
         <v>7</v>
@@ -3902,7 +3898,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3919,19 +3915,19 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>445</v>
+      </c>
+      <c r="D1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>11</v>
-      </c>
-      <c r="E1" t="s">
-        <v>12</v>
       </c>
       <c r="F1" t="s">
         <v>6</v>
@@ -3940,7 +3936,7 @@
         <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -3948,25 +3944,25 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E2" t="s">
+        <v>125</v>
+      </c>
+      <c r="F2" t="s">
         <v>126</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>127</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>128</v>
-      </c>
-      <c r="G2" t="s">
-        <v>129</v>
-      </c>
-      <c r="H2" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -3974,25 +3970,25 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
+        <v>130</v>
+      </c>
+      <c r="E3" t="s">
+        <v>131</v>
+      </c>
+      <c r="F3" t="s">
         <v>132</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>133</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>134</v>
-      </c>
-      <c r="G3" t="s">
-        <v>135</v>
-      </c>
-      <c r="H3" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -4000,25 +3996,25 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C4">
         <v>2</v>
       </c>
       <c r="D4" t="s">
+        <v>136</v>
+      </c>
+      <c r="E4" t="s">
+        <v>137</v>
+      </c>
+      <c r="F4" t="s">
         <v>138</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
         <v>139</v>
       </c>
-      <c r="F4" t="s">
+      <c r="H4" t="s">
         <v>140</v>
-      </c>
-      <c r="G4" t="s">
-        <v>141</v>
-      </c>
-      <c r="H4" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -4026,25 +4022,25 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C5">
         <v>2</v>
       </c>
       <c r="D5" t="s">
+        <v>142</v>
+      </c>
+      <c r="E5" t="s">
+        <v>143</v>
+      </c>
+      <c r="F5" t="s">
         <v>144</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>145</v>
       </c>
-      <c r="F5" t="s">
-        <v>146</v>
-      </c>
-      <c r="G5" t="s">
-        <v>147</v>
-      </c>
       <c r="H5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -4052,25 +4048,25 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C6">
         <v>3</v>
       </c>
       <c r="D6" t="s">
+        <v>147</v>
+      </c>
+      <c r="E6" t="s">
+        <v>148</v>
+      </c>
+      <c r="F6" t="s">
         <v>149</v>
       </c>
-      <c r="E6" t="s">
+      <c r="G6" t="s">
         <v>150</v>
       </c>
-      <c r="F6" t="s">
-        <v>151</v>
-      </c>
-      <c r="G6" t="s">
-        <v>152</v>
-      </c>
       <c r="H6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -4078,25 +4074,25 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C7">
         <v>4</v>
       </c>
       <c r="D7" t="s">
+        <v>152</v>
+      </c>
+      <c r="E7" t="s">
+        <v>153</v>
+      </c>
+      <c r="F7" t="s">
         <v>154</v>
       </c>
-      <c r="E7" t="s">
+      <c r="G7" t="s">
         <v>155</v>
       </c>
-      <c r="F7" t="s">
-        <v>156</v>
-      </c>
-      <c r="G7" t="s">
-        <v>157</v>
-      </c>
       <c r="H7" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -4104,25 +4100,25 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C8">
         <v>5</v>
       </c>
       <c r="D8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E8" t="s">
+        <v>158</v>
+      </c>
+      <c r="F8" t="s">
         <v>159</v>
       </c>
-      <c r="E8" t="s">
+      <c r="G8" t="s">
         <v>160</v>
       </c>
-      <c r="F8" t="s">
-        <v>161</v>
-      </c>
-      <c r="G8" t="s">
-        <v>162</v>
-      </c>
       <c r="H8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -4130,25 +4126,25 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C9">
         <v>6</v>
       </c>
       <c r="D9" t="s">
+        <v>162</v>
+      </c>
+      <c r="E9" t="s">
+        <v>163</v>
+      </c>
+      <c r="F9" t="s">
         <v>164</v>
       </c>
-      <c r="E9" t="s">
+      <c r="G9" t="s">
         <v>165</v>
       </c>
-      <c r="F9" t="s">
-        <v>166</v>
-      </c>
-      <c r="G9" t="s">
-        <v>167</v>
-      </c>
       <c r="H9" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -4156,25 +4152,25 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C10">
         <v>7</v>
       </c>
       <c r="D10" t="s">
+        <v>167</v>
+      </c>
+      <c r="E10" t="s">
+        <v>168</v>
+      </c>
+      <c r="F10" t="s">
         <v>169</v>
       </c>
-      <c r="E10" t="s">
+      <c r="G10" t="s">
         <v>170</v>
       </c>
-      <c r="F10" t="s">
-        <v>171</v>
-      </c>
-      <c r="G10" t="s">
-        <v>172</v>
-      </c>
       <c r="H10" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -4182,25 +4178,25 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C11">
         <v>8</v>
       </c>
       <c r="D11" t="s">
+        <v>172</v>
+      </c>
+      <c r="E11" t="s">
+        <v>173</v>
+      </c>
+      <c r="F11" t="s">
         <v>174</v>
       </c>
-      <c r="E11" t="s">
+      <c r="G11" t="s">
         <v>175</v>
       </c>
-      <c r="F11" t="s">
-        <v>176</v>
-      </c>
-      <c r="G11" t="s">
-        <v>177</v>
-      </c>
       <c r="H11" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -4230,19 +4226,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>15</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>17</v>
-      </c>
-      <c r="E1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -4250,16 +4246,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -4267,16 +4263,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D3">
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -4284,16 +4280,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D4">
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -4301,16 +4297,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D5">
         <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -4318,16 +4314,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C6" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D6">
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -4335,16 +4331,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C7" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D7">
         <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -4352,16 +4348,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C8" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D8">
         <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -4369,16 +4365,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C9" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D9">
         <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -4386,16 +4382,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C10" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D10">
         <v>9</v>
       </c>
       <c r="E10" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -4403,16 +4399,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C11" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D11">
         <v>10</v>
       </c>
       <c r="E11" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -4442,10 +4438,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
         <v>5</v>
@@ -4454,7 +4450,7 @@
         <v>6</v>
       </c>
       <c r="E1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -4462,16 +4458,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C2" t="s">
+        <v>199</v>
+      </c>
+      <c r="D2" t="s">
         <v>200</v>
       </c>
-      <c r="C2" t="s">
-        <v>201</v>
-      </c>
-      <c r="D2" t="s">
-        <v>202</v>
-      </c>
       <c r="E2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -4479,16 +4475,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C3" t="s">
+        <v>202</v>
+      </c>
+      <c r="D3" t="s">
         <v>203</v>
       </c>
-      <c r="C3" t="s">
-        <v>204</v>
-      </c>
-      <c r="D3" t="s">
-        <v>205</v>
-      </c>
       <c r="E3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -4496,16 +4492,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>204</v>
+      </c>
+      <c r="C4" t="s">
+        <v>205</v>
+      </c>
+      <c r="D4" t="s">
         <v>206</v>
       </c>
-      <c r="C4" t="s">
-        <v>207</v>
-      </c>
-      <c r="D4" t="s">
-        <v>208</v>
-      </c>
       <c r="E4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -4513,16 +4509,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>207</v>
+      </c>
+      <c r="C5" t="s">
+        <v>208</v>
+      </c>
+      <c r="D5" t="s">
         <v>209</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
         <v>210</v>
-      </c>
-      <c r="D5" t="s">
-        <v>211</v>
-      </c>
-      <c r="E5" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -4530,16 +4526,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>211</v>
+      </c>
+      <c r="C6" t="s">
+        <v>212</v>
+      </c>
+      <c r="D6" t="s">
         <v>213</v>
       </c>
-      <c r="C6" t="s">
+      <c r="E6" t="s">
         <v>214</v>
-      </c>
-      <c r="D6" t="s">
-        <v>215</v>
-      </c>
-      <c r="E6" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -4547,16 +4543,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>215</v>
+      </c>
+      <c r="C7" t="s">
+        <v>216</v>
+      </c>
+      <c r="D7" t="s">
         <v>217</v>
       </c>
-      <c r="C7" t="s">
-        <v>218</v>
-      </c>
-      <c r="D7" t="s">
-        <v>219</v>
-      </c>
       <c r="E7" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -4564,16 +4560,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>218</v>
+      </c>
+      <c r="C8" t="s">
+        <v>219</v>
+      </c>
+      <c r="D8" t="s">
         <v>220</v>
       </c>
-      <c r="C8" t="s">
+      <c r="E8" t="s">
         <v>221</v>
-      </c>
-      <c r="D8" t="s">
-        <v>222</v>
-      </c>
-      <c r="E8" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -4581,16 +4577,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>222</v>
+      </c>
+      <c r="C9" t="s">
+        <v>223</v>
+      </c>
+      <c r="D9" t="s">
         <v>224</v>
       </c>
-      <c r="C9" t="s">
-        <v>225</v>
-      </c>
-      <c r="D9" t="s">
-        <v>226</v>
-      </c>
       <c r="E9" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -4598,16 +4594,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>225</v>
+      </c>
+      <c r="C10" t="s">
+        <v>226</v>
+      </c>
+      <c r="D10" t="s">
         <v>227</v>
       </c>
-      <c r="C10" t="s">
+      <c r="E10" t="s">
         <v>228</v>
-      </c>
-      <c r="D10" t="s">
-        <v>229</v>
-      </c>
-      <c r="E10" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -4615,16 +4611,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>229</v>
+      </c>
+      <c r="C11" t="s">
+        <v>230</v>
+      </c>
+      <c r="D11" t="s">
         <v>231</v>
       </c>
-      <c r="C11" t="s">
+      <c r="E11" t="s">
         <v>232</v>
-      </c>
-      <c r="D11" t="s">
-        <v>233</v>
-      </c>
-      <c r="E11" t="s">
-        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -4637,10 +4633,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AFA39DB-A819-4313-9DED-12F488258F9C}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4653,40 +4649,44 @@
     <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
         <v>20</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>21</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>445</v>
+      </c>
+      <c r="E1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>23</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>24</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>25</v>
       </c>
-      <c r="G1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -4698,21 +4698,24 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="G2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="H2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -4724,21 +4727,24 @@
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="G3" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="H3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -4750,21 +4756,24 @@
         <v>3</v>
       </c>
       <c r="F4" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="G4" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="H4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -4776,21 +4785,24 @@
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="G5" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="H5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -4802,21 +4814,24 @@
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G6" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="H6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C7">
         <v>6</v>
@@ -4828,21 +4843,24 @@
         <v>4</v>
       </c>
       <c r="F7" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="G7" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="H7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -4854,21 +4872,24 @@
         <v>3</v>
       </c>
       <c r="F8" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="G8" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="H8">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C9">
         <v>8</v>
@@ -4880,21 +4901,24 @@
         <v>2</v>
       </c>
       <c r="F9" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="G9" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="H9">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C10">
         <v>9</v>
@@ -4906,21 +4930,24 @@
         <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="G10" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="H10">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C11">
         <v>10</v>
@@ -4932,12 +4959,15 @@
         <v>3</v>
       </c>
       <c r="F11" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="G11" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="H11">
+        <v>10</v>
+      </c>
+      <c r="I11">
         <v>10</v>
       </c>
     </row>
@@ -4969,22 +4999,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
         <v>28</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>29</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>30</v>
       </c>
-      <c r="D1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" t="s">
-        <v>32</v>
-      </c>
       <c r="F1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -4992,10 +5022,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D2">
         <v>40</v>
@@ -5012,10 +5042,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C3" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D3">
         <v>30</v>
@@ -5032,10 +5062,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C4" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D4">
         <v>60</v>
@@ -5052,10 +5082,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C5" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D5">
         <v>15</v>
@@ -5072,10 +5102,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C6" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D6">
         <v>60</v>
@@ -5092,10 +5122,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C7" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D7">
         <v>45</v>
@@ -5112,10 +5142,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C8" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D8">
         <v>30</v>
@@ -5132,10 +5162,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C9" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D9">
         <v>50</v>
@@ -5152,10 +5182,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C10" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D10">
         <v>90</v>
@@ -5172,10 +5202,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C11" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D11">
         <v>60</v>
@@ -5213,16 +5243,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
         <v>30</v>
-      </c>
-      <c r="D1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -5230,10 +5260,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -5244,10 +5274,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C3" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -5258,10 +5288,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C4" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -5272,10 +5302,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C5" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -5286,10 +5316,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C6" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -5300,10 +5330,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C7" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D7">
         <v>4</v>
@@ -5314,10 +5344,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C8" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D8">
         <v>4</v>
@@ -5328,10 +5358,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C9" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D9">
         <v>3</v>
@@ -5342,10 +5372,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C10" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D10">
         <v>5</v>
@@ -5356,10 +5386,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C11" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -5392,25 +5422,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
         <v>34</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>35</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>36</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" t="s">
         <v>37</v>
-      </c>
-      <c r="E1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -5430,7 +5460,7 @@
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -5450,7 +5480,7 @@
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -5470,7 +5500,7 @@
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -5487,10 +5517,10 @@
         <v>59.13</v>
       </c>
       <c r="E5" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -5510,7 +5540,7 @@
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -5527,10 +5557,10 @@
         <v>93.89</v>
       </c>
       <c r="E7" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F7" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -5547,10 +5577,10 @@
         <v>183.5</v>
       </c>
       <c r="E8" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F8" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -5567,10 +5597,10 @@
         <v>138.79</v>
       </c>
       <c r="E9" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F9" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -5587,10 +5617,10 @@
         <v>177.8</v>
       </c>
       <c r="E10" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F10" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -5607,10 +5637,10 @@
         <v>193.85</v>
       </c>
       <c r="E11" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F11" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
   </sheetData>
@@ -5645,22 +5675,22 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
         <v>40</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>41</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>42</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>43</v>
-      </c>
-      <c r="F1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -5668,19 +5698,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>304</v>
+      </c>
+      <c r="C2" t="s">
+        <v>305</v>
+      </c>
+      <c r="D2" t="s">
         <v>306</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>307</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>308</v>
-      </c>
-      <c r="E2" t="s">
-        <v>309</v>
-      </c>
-      <c r="F2" t="s">
-        <v>310</v>
       </c>
       <c r="G2">
         <v>240</v>
@@ -5691,19 +5721,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>309</v>
+      </c>
+      <c r="C3" t="s">
+        <v>310</v>
+      </c>
+      <c r="D3" t="s">
         <v>311</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
+        <v>307</v>
+      </c>
+      <c r="F3" t="s">
         <v>312</v>
-      </c>
-      <c r="D3" t="s">
-        <v>313</v>
-      </c>
-      <c r="E3" t="s">
-        <v>309</v>
-      </c>
-      <c r="F3" t="s">
-        <v>314</v>
       </c>
       <c r="G3">
         <v>116</v>
@@ -5714,19 +5744,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>313</v>
+      </c>
+      <c r="C4" t="s">
+        <v>314</v>
+      </c>
+      <c r="D4" t="s">
         <v>315</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
+        <v>307</v>
+      </c>
+      <c r="F4" t="s">
         <v>316</v>
-      </c>
-      <c r="D4" t="s">
-        <v>317</v>
-      </c>
-      <c r="E4" t="s">
-        <v>309</v>
-      </c>
-      <c r="F4" t="s">
-        <v>318</v>
       </c>
       <c r="G4">
         <v>636</v>
@@ -5737,19 +5767,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>317</v>
+      </c>
+      <c r="C5" t="s">
+        <v>318</v>
+      </c>
+      <c r="D5" t="s">
         <v>319</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
+        <v>307</v>
+      </c>
+      <c r="F5" t="s">
         <v>320</v>
-      </c>
-      <c r="D5" t="s">
-        <v>321</v>
-      </c>
-      <c r="E5" t="s">
-        <v>309</v>
-      </c>
-      <c r="F5" t="s">
-        <v>322</v>
       </c>
       <c r="G5">
         <v>626</v>
@@ -5760,19 +5790,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>321</v>
+      </c>
+      <c r="C6" t="s">
+        <v>322</v>
+      </c>
+      <c r="D6" t="s">
         <v>323</v>
       </c>
-      <c r="C6" t="s">
+      <c r="E6" t="s">
+        <v>307</v>
+      </c>
+      <c r="F6" t="s">
         <v>324</v>
-      </c>
-      <c r="D6" t="s">
-        <v>325</v>
-      </c>
-      <c r="E6" t="s">
-        <v>309</v>
-      </c>
-      <c r="F6" t="s">
-        <v>326</v>
       </c>
       <c r="G6">
         <v>833</v>
@@ -5783,19 +5813,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>325</v>
+      </c>
+      <c r="C7" t="s">
+        <v>326</v>
+      </c>
+      <c r="D7" t="s">
         <v>327</v>
       </c>
-      <c r="C7" t="s">
+      <c r="E7" t="s">
+        <v>307</v>
+      </c>
+      <c r="F7" t="s">
         <v>328</v>
-      </c>
-      <c r="D7" t="s">
-        <v>329</v>
-      </c>
-      <c r="E7" t="s">
-        <v>309</v>
-      </c>
-      <c r="F7" t="s">
-        <v>330</v>
       </c>
       <c r="G7">
         <v>218</v>
@@ -5806,19 +5836,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>329</v>
+      </c>
+      <c r="C8" t="s">
+        <v>330</v>
+      </c>
+      <c r="D8" t="s">
         <v>331</v>
       </c>
-      <c r="C8" t="s">
+      <c r="E8" t="s">
+        <v>307</v>
+      </c>
+      <c r="F8" t="s">
         <v>332</v>
-      </c>
-      <c r="D8" t="s">
-        <v>333</v>
-      </c>
-      <c r="E8" t="s">
-        <v>309</v>
-      </c>
-      <c r="F8" t="s">
-        <v>334</v>
       </c>
       <c r="G8">
         <v>18</v>
@@ -5829,19 +5859,19 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>333</v>
+      </c>
+      <c r="C9" t="s">
+        <v>334</v>
+      </c>
+      <c r="D9" t="s">
         <v>335</v>
       </c>
-      <c r="C9" t="s">
+      <c r="E9" t="s">
+        <v>307</v>
+      </c>
+      <c r="F9" t="s">
         <v>336</v>
-      </c>
-      <c r="D9" t="s">
-        <v>337</v>
-      </c>
-      <c r="E9" t="s">
-        <v>309</v>
-      </c>
-      <c r="F9" t="s">
-        <v>338</v>
       </c>
       <c r="G9">
         <v>932</v>
@@ -5852,19 +5882,19 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>337</v>
+      </c>
+      <c r="C10" t="s">
+        <v>338</v>
+      </c>
+      <c r="D10" t="s">
         <v>339</v>
       </c>
-      <c r="C10" t="s">
+      <c r="E10" t="s">
+        <v>307</v>
+      </c>
+      <c r="F10" t="s">
         <v>340</v>
-      </c>
-      <c r="D10" t="s">
-        <v>341</v>
-      </c>
-      <c r="E10" t="s">
-        <v>309</v>
-      </c>
-      <c r="F10" t="s">
-        <v>342</v>
       </c>
       <c r="G10">
         <v>655</v>
@@ -5875,19 +5905,19 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>341</v>
+      </c>
+      <c r="C11" t="s">
+        <v>342</v>
+      </c>
+      <c r="D11" t="s">
         <v>343</v>
       </c>
-      <c r="C11" t="s">
+      <c r="E11" t="s">
+        <v>307</v>
+      </c>
+      <c r="F11" t="s">
         <v>344</v>
-      </c>
-      <c r="D11" t="s">
-        <v>345</v>
-      </c>
-      <c r="E11" t="s">
-        <v>309</v>
-      </c>
-      <c r="F11" t="s">
-        <v>346</v>
       </c>
       <c r="G11">
         <v>777</v>

</xml_diff>